<commit_message>
Updated delta wavelengths, and csv metadata.
</commit_message>
<xml_diff>
--- a/kyton_out.xlsx
+++ b/kyton_out.xlsx
@@ -957,79 +957,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>-0.01500000007581548</c:v>
+                  <c:v>-2.273736754432321e-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.1549999997223495</c:v>
+                  <c:v>-0.1399999998739077</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.6399999999757711</c:v>
+                  <c:v>-0.6250000001273293</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.529999999798747</c:v>
+                  <c:v>-0.5149999999503052</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.4300000000512227</c:v>
+                  <c:v>-0.4150000002027809</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.5349999996724364</c:v>
+                  <c:v>-0.5199999998239946</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.7849999997233681</c:v>
+                  <c:v>-0.7699999998749263</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.7000000000516593</c:v>
+                  <c:v>-0.6850000002032175</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.4149999999754073</c:v>
+                  <c:v>-0.4000000001269655</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.1449999999749707</c:v>
+                  <c:v>-0.1300000001265289</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.2399999998488056</c:v>
+                  <c:v>-0.2250000000003638</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.244999999722495</c:v>
+                  <c:v>-0.2299999998740532</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.3999999998995918</c:v>
+                  <c:v>-0.38500000005115</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.7100000000264117</c:v>
+                  <c:v>0.7249999998748535</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.4250000001775334</c:v>
+                  <c:v>0.4400000000259752</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.4250000001775334</c:v>
+                  <c:v>0.4400000000259752</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.7800000003044261</c:v>
+                  <c:v>0.7950000001528679</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.9050000001025182</c:v>
+                  <c:v>0.91999999995096</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.150000000052387</c:v>
+                  <c:v>1.164999999900829</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.23000000007778</c:v>
+                  <c:v>1.244999999926222</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.8550000002287561</c:v>
+                  <c:v>0.8700000000771979</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.085000000330183</c:v>
+                  <c:v>1.100000000178625</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.8550000002287561</c:v>
+                  <c:v>0.8700000000771979</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.6800000001021544</c:v>
+                  <c:v>0.6949999999505962</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.4149999999754073</c:v>
+                  <c:v>0.4299999998238491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1087,7 +1087,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Δ average (pm)</a:t>
+                  <a:t>Δλ average (pm)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1532,22 +1532,22 @@
         <v>522.0899999999999</v>
       </c>
       <c r="L2">
-        <v>0.6224500000000717</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>3.184650000000147</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>-1.285329999999931</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>-2.521829999999909</v>
+        <v>0</v>
       </c>
       <c r="P2" s="11">
         <v>0.01499999999987267</v>
       </c>
       <c r="Q2">
-        <v>-0.01500000007581548</v>
+        <v>-2.273736754432321e-10</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1585,22 +1585,22 @@
         <v>522.0694999999999</v>
       </c>
       <c r="L3">
-        <v>0.6227499999999964</v>
+        <v>0.0002999999999246938</v>
       </c>
       <c r="M3">
-        <v>3.18387000000007</v>
+        <v>-0.0007800000000770524</v>
       </c>
       <c r="N3">
-        <v>-1.284849999999778</v>
+        <v>0.0004800000001523586</v>
       </c>
       <c r="O3">
-        <v>-2.522389999999859</v>
+        <v>-0.000559999999950378</v>
       </c>
       <c r="P3" s="11">
         <v>-0.005500000000097316</v>
       </c>
       <c r="Q3">
-        <v>-0.1549999997223495</v>
+        <v>-0.1399999998739077</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1638,22 +1638,22 @@
         <v>522.067</v>
       </c>
       <c r="L4">
-        <v>0.6223100000001978</v>
+        <v>-0.0001399999998739077</v>
       </c>
       <c r="M4">
-        <v>3.183590000000095</v>
+        <v>-0.001060000000052241</v>
       </c>
       <c r="N4">
-        <v>-1.285149999999931</v>
+        <v>0.000180000000000291</v>
       </c>
       <c r="O4">
-        <v>-2.52330999999981</v>
+        <v>-0.001479999999901338</v>
       </c>
       <c r="P4" s="11">
         <v>-0.008000000000038199</v>
       </c>
       <c r="Q4">
-        <v>-0.6399999999757711</v>
+        <v>-0.6250000001273293</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1691,22 +1691,22 @@
         <v>522.066</v>
       </c>
       <c r="L5">
-        <v>0.6224100000001727</v>
+        <v>-3.999999989900971e-05</v>
       </c>
       <c r="M5">
-        <v>3.183590000000095</v>
+        <v>-0.001060000000052241</v>
       </c>
       <c r="N5">
-        <v>-1.28536999999983</v>
+        <v>-3.999999989900971e-05</v>
       </c>
       <c r="O5">
-        <v>-2.52274999999986</v>
+        <v>-0.00091999999995096</v>
       </c>
       <c r="P5" s="11">
         <v>-0.009000000000014552</v>
       </c>
       <c r="Q5">
-        <v>-0.529999999798747</v>
+        <v>-0.5149999999503052</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1744,22 +1744,22 @@
         <v>522.0649999999999</v>
       </c>
       <c r="L6">
-        <v>0.6224100000001727</v>
+        <v>-3.999999989900971e-05</v>
       </c>
       <c r="M6">
-        <v>3.184110000000146</v>
+        <v>-0.0005400000000008731</v>
       </c>
       <c r="N6">
-        <v>-1.285649999999805</v>
+        <v>-0.0003199999998741987</v>
       </c>
       <c r="O6">
-        <v>-2.522589999999809</v>
+        <v>-0.0007599999999001739</v>
       </c>
       <c r="P6" s="11">
         <v>-0.01000000000010459</v>
       </c>
       <c r="Q6">
-        <v>-0.4300000000512227</v>
+        <v>-0.4150000002027809</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1797,22 +1797,22 @@
         <v>522.0654999999999</v>
       </c>
       <c r="L7">
-        <v>0.6221700000000965</v>
+        <v>-0.000279999999975189</v>
       </c>
       <c r="M7">
-        <v>3.184290000000146</v>
+        <v>-0.0003600000000005821</v>
       </c>
       <c r="N7">
-        <v>-1.28572999999983</v>
+        <v>-0.0003999999998995918</v>
       </c>
       <c r="O7">
-        <v>-2.522869999999784</v>
+        <v>-0.001039999999875363</v>
       </c>
       <c r="P7" s="11">
         <v>-0.009500000000116415</v>
       </c>
       <c r="Q7">
-        <v>-0.5349999996724364</v>
+        <v>-0.5199999998239946</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1850,22 +1850,22 @@
         <v>522.064</v>
       </c>
       <c r="L8">
-        <v>0.6219300000000203</v>
+        <v>-0.0005200000000513683</v>
       </c>
       <c r="M8">
-        <v>3.183430000000044</v>
+        <v>-0.001220000000103028</v>
       </c>
       <c r="N8">
-        <v>-1.28534999999988</v>
+        <v>-1.999999994950485e-05</v>
       </c>
       <c r="O8">
-        <v>-2.523149999999987</v>
+        <v>-0.001320000000077926</v>
       </c>
       <c r="P8" s="11">
         <v>-0.01100000000008095</v>
       </c>
       <c r="Q8">
-        <v>-0.7849999997233681</v>
+        <v>-0.7699999998749263</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1903,22 +1903,22 @@
         <v>522.064</v>
       </c>
       <c r="L9">
-        <v>0.6220900000000711</v>
+        <v>-0.0003600000000005821</v>
       </c>
       <c r="M9">
-        <v>3.184470000000147</v>
+        <v>-0.000180000000000291</v>
       </c>
       <c r="N9">
-        <v>-1.286169999999856</v>
+        <v>-0.000839999999925567</v>
       </c>
       <c r="O9">
-        <v>-2.523189999999886</v>
+        <v>-0.001359999999976935</v>
       </c>
       <c r="P9" s="11">
         <v>-0.01100000000008095</v>
       </c>
       <c r="Q9">
-        <v>-0.7000000000516593</v>
+        <v>-0.6850000002032175</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1956,22 +1956,22 @@
         <v>522.0675</v>
       </c>
       <c r="L10">
-        <v>0.6223899999999958</v>
+        <v>-6.000000007588824e-05</v>
       </c>
       <c r="M10">
-        <v>3.184150000000045</v>
+        <v>-0.0005000000001018634</v>
       </c>
       <c r="N10">
-        <v>-1.285449999999855</v>
+        <v>-0.0001199999999244028</v>
       </c>
       <c r="O10">
-        <v>-2.52274999999986</v>
+        <v>-0.00091999999995096</v>
       </c>
       <c r="P10" s="11">
         <v>-0.007500000000050022</v>
       </c>
       <c r="Q10">
-        <v>-0.4149999999754073</v>
+        <v>-0.4000000001269655</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2009,22 +2009,22 @@
         <v>522.0685</v>
       </c>
       <c r="L11">
-        <v>0.6227700000001732</v>
+        <v>0.0003200000001015724</v>
       </c>
       <c r="M11">
-        <v>3.184390000000121</v>
+        <v>-0.0002600000000256841</v>
       </c>
       <c r="N11">
-        <v>-1.285449999999855</v>
+        <v>-0.0001199999999244028</v>
       </c>
       <c r="O11">
-        <v>-2.522289999999884</v>
+        <v>-0.00045999999997548</v>
       </c>
       <c r="P11" s="11">
         <v>-0.006500000000073669</v>
       </c>
       <c r="Q11">
-        <v>-0.1449999999749707</v>
+        <v>-0.1300000001265289</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2062,22 +2062,22 @@
         <v>522.072</v>
       </c>
       <c r="L12">
-        <v>0.6227900000001227</v>
+        <v>0.0003400000000510772</v>
       </c>
       <c r="M12">
-        <v>3.184150000000045</v>
+        <v>-0.0005000000001018634</v>
       </c>
       <c r="N12">
-        <v>-1.285449999999855</v>
+        <v>-0.0001199999999244028</v>
       </c>
       <c r="O12">
-        <v>-2.522449999999935</v>
+        <v>-0.0006200000000262662</v>
       </c>
       <c r="P12" s="11">
         <v>-0.003000000000042746</v>
       </c>
       <c r="Q12">
-        <v>-0.2399999998488056</v>
+        <v>-0.2250000000003638</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2115,22 +2115,22 @@
         <v>522.0735</v>
       </c>
       <c r="L13">
-        <v>0.6223700000000463</v>
+        <v>-8.000000002539309e-05</v>
       </c>
       <c r="M13">
-        <v>3.184370000000172</v>
+        <v>-0.000279999999975189</v>
       </c>
       <c r="N13">
-        <v>-1.285389999999779</v>
+        <v>-5.999999984851456e-05</v>
       </c>
       <c r="O13">
-        <v>-2.522329999999783</v>
+        <v>-0.0004999999998744897</v>
       </c>
       <c r="P13" s="11">
         <v>-0.001500000000078217</v>
       </c>
       <c r="Q13">
-        <v>-0.244999999722495</v>
+        <v>-0.2299999998740532</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -2168,22 +2168,22 @@
         <v>522.075</v>
       </c>
       <c r="L14">
-        <v>0.622630000000072</v>
+        <v>0.000180000000000291</v>
       </c>
       <c r="M14">
-        <v>3.184570000000122</v>
+        <v>-8.000000002539309e-05</v>
       </c>
       <c r="N14">
-        <v>-1.285509999999931</v>
+        <v>-0.000180000000000291</v>
       </c>
       <c r="O14">
-        <v>-2.523289999999861</v>
+        <v>-0.001459999999951833</v>
       </c>
       <c r="P14" s="11">
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>-0.3999999998995918</v>
+        <v>-0.38500000005115</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2221,22 +2221,22 @@
         <v>522.1105</v>
       </c>
       <c r="L15">
-        <v>0.6232700000000477</v>
+        <v>0.0008199999999760621</v>
       </c>
       <c r="M15">
-        <v>3.185010000000148</v>
+        <v>0.0003600000000005821</v>
       </c>
       <c r="N15">
-        <v>-1.283950000000004</v>
+        <v>0.00137999999992644</v>
       </c>
       <c r="O15">
-        <v>-2.521489999999858</v>
+        <v>0.0003400000000510772</v>
       </c>
       <c r="P15" s="11">
         <v>0.03549999999995634</v>
       </c>
       <c r="Q15">
-        <v>0.7100000000264117</v>
+        <v>0.7249999998748535</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2274,22 +2274,22 @@
         <v>522.1134999999999</v>
       </c>
       <c r="L16">
-        <v>0.6238299999999981</v>
+        <v>0.00137999999992644</v>
       </c>
       <c r="M16">
-        <v>3.184810000000198</v>
+        <v>0.0001600000000507862</v>
       </c>
       <c r="N16">
-        <v>-1.284729999999854</v>
+        <v>0.0006000000000767614</v>
       </c>
       <c r="O16">
-        <v>-2.522209999999859</v>
+        <v>-0.0003799999999500869</v>
       </c>
       <c r="P16" s="11">
         <v>0.0384999999998854</v>
       </c>
       <c r="Q16">
-        <v>0.4250000001775334</v>
+        <v>0.4400000000259752</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2327,22 +2327,22 @@
         <v>522.1134999999999</v>
       </c>
       <c r="L17">
-        <v>0.6234900000001744</v>
+        <v>0.001040000000102737</v>
       </c>
       <c r="M17">
-        <v>3.184709999999995</v>
+        <v>5.999999984851456e-05</v>
       </c>
       <c r="N17">
-        <v>-1.284049999999979</v>
+        <v>0.001279999999951542</v>
       </c>
       <c r="O17">
-        <v>-2.522449999999935</v>
+        <v>-0.0006200000000262662</v>
       </c>
       <c r="P17" s="11">
         <v>0.0384999999998854</v>
       </c>
       <c r="Q17">
-        <v>0.4250000001775334</v>
+        <v>0.4400000000259752</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2380,22 +2380,22 @@
         <v>522.1129999999999</v>
       </c>
       <c r="L18">
-        <v>0.6236700000001747</v>
+        <v>0.001220000000103028</v>
       </c>
       <c r="M18">
-        <v>3.185530000000199</v>
+        <v>0.0008800000000519503</v>
       </c>
       <c r="N18">
-        <v>-1.284549999999854</v>
+        <v>0.0007800000000770524</v>
       </c>
       <c r="O18">
-        <v>-2.521529999999984</v>
+        <v>0.0002999999999246938</v>
       </c>
       <c r="P18" s="11">
         <v>0.03799999999989723</v>
       </c>
       <c r="Q18">
-        <v>0.7800000003044261</v>
+        <v>0.7950000001528679</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2433,22 +2433,22 @@
         <v>522.1129999999999</v>
       </c>
       <c r="L19">
-        <v>0.6238100000000486</v>
+        <v>0.001359999999976935</v>
       </c>
       <c r="M19">
-        <v>3.185190000000148</v>
+        <v>0.0005400000000008731</v>
       </c>
       <c r="N19">
-        <v>-1.284109999999828</v>
+        <v>0.001220000000103028</v>
       </c>
       <c r="O19">
-        <v>-2.521269999999959</v>
+        <v>0.000559999999950378</v>
       </c>
       <c r="P19" s="11">
         <v>0.03799999999989723</v>
       </c>
       <c r="Q19">
-        <v>0.9050000001025182</v>
+        <v>0.91999999995096</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -2486,22 +2486,22 @@
         <v>522.114</v>
       </c>
       <c r="L20">
-        <v>0.6240500000001248</v>
+        <v>0.001600000000053114</v>
       </c>
       <c r="M20">
-        <v>3.185170000000198</v>
+        <v>0.0005200000000513683</v>
       </c>
       <c r="N20">
-        <v>-1.283829999999853</v>
+        <v>0.001500000000078217</v>
       </c>
       <c r="O20">
-        <v>-2.520789999999806</v>
+        <v>0.001040000000102737</v>
       </c>
       <c r="P20" s="11">
         <v>0.03899999999998727</v>
       </c>
       <c r="Q20">
-        <v>1.150000000052387</v>
+        <v>1.164999999900829</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2539,22 +2539,22 @@
         <v>522.1165</v>
       </c>
       <c r="L21">
-        <v>0.6239300000002004</v>
+        <v>0.001480000000128712</v>
       </c>
       <c r="M21">
-        <v>3.185969999999998</v>
+        <v>0.001319999999850552</v>
       </c>
       <c r="N21">
-        <v>-1.284289999999828</v>
+        <v>0.001040000000102737</v>
       </c>
       <c r="O21">
-        <v>-2.520689999999831</v>
+        <v>0.001140000000077634</v>
       </c>
       <c r="P21" s="11">
         <v>0.04149999999992815</v>
       </c>
       <c r="Q21">
-        <v>1.23000000007778</v>
+        <v>1.244999999926222</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -2592,22 +2592,22 @@
         <v>522.1185</v>
       </c>
       <c r="L22">
-        <v>0.6239300000002004</v>
+        <v>0.001480000000128712</v>
       </c>
       <c r="M22">
-        <v>3.185570000000098</v>
+        <v>0.00091999999995096</v>
       </c>
       <c r="N22">
-        <v>-1.284369999999853</v>
+        <v>0.0009600000000773434</v>
       </c>
       <c r="O22">
-        <v>-2.521709999999985</v>
+        <v>0.0001199999999244028</v>
       </c>
       <c r="P22" s="11">
         <v>0.04349999999999454</v>
       </c>
       <c r="Q22">
-        <v>0.8550000002287561</v>
+        <v>0.8700000000771979</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2645,22 +2645,22 @@
         <v>522.1189999999999</v>
       </c>
       <c r="L23">
-        <v>0.6244100000001254</v>
+        <v>0.001960000000053697</v>
       </c>
       <c r="M23">
-        <v>3.185850000000073</v>
+        <v>0.001199999999926149</v>
       </c>
       <c r="N23">
-        <v>-1.284029999999802</v>
+        <v>0.001300000000128421</v>
       </c>
       <c r="O23">
-        <v>-2.521889999999985</v>
+        <v>-6.000000007588824e-05</v>
       </c>
       <c r="P23" s="11">
         <v>0.04399999999986903</v>
       </c>
       <c r="Q23">
-        <v>1.085000000330183</v>
+        <v>1.100000000178625</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2698,22 +2698,22 @@
         <v>522.1195</v>
       </c>
       <c r="L24">
-        <v>0.6231700000000728</v>
+        <v>0.0007200000000011642</v>
       </c>
       <c r="M24">
-        <v>3.185210000000097</v>
+        <v>0.000559999999950378</v>
       </c>
       <c r="N24">
-        <v>-1.284329999999954</v>
+        <v>0.0009999999999763531</v>
       </c>
       <c r="O24">
-        <v>-2.520629999999983</v>
+        <v>0.001199999999926149</v>
       </c>
       <c r="P24" s="11">
         <v>0.0444999999999709</v>
       </c>
       <c r="Q24">
-        <v>0.8550000002287561</v>
+        <v>0.8700000000771979</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2751,22 +2751,22 @@
         <v>522.122</v>
       </c>
       <c r="L25">
-        <v>0.6237100000000737</v>
+        <v>0.001260000000002037</v>
       </c>
       <c r="M25">
-        <v>3.185290000000123</v>
+        <v>0.0006399999999757711</v>
       </c>
       <c r="N25">
-        <v>-1.284429999999929</v>
+        <v>0.0009000000000014552</v>
       </c>
       <c r="O25">
-        <v>-2.521849999999858</v>
+        <v>-1.999999994950485e-05</v>
       </c>
       <c r="P25" s="11">
         <v>0.04699999999991178</v>
       </c>
       <c r="Q25">
-        <v>0.6800000001021544</v>
+        <v>0.6949999999505962</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2804,22 +2804,22 @@
         <v>522.1285</v>
       </c>
       <c r="L26">
-        <v>0.6236700000001747</v>
+        <v>0.001220000000103028</v>
       </c>
       <c r="M26">
-        <v>3.184970000000021</v>
+        <v>0.0003199999998741987</v>
       </c>
       <c r="N26">
-        <v>-1.284729999999854</v>
+        <v>0.0006000000000767614</v>
       </c>
       <c r="O26">
-        <v>-2.522249999999985</v>
+        <v>-0.0004200000000764703</v>
       </c>
       <c r="P26" s="11">
         <v>0.05349999999998545</v>
       </c>
       <c r="Q26">
-        <v>0.4149999999754073</v>
+        <v>0.4299999998238491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated fiber finder algorithm, and UI aesthetics.
</commit_message>
<xml_diff>
--- a/kyton_out.xlsx
+++ b/kyton_out.xlsx
@@ -40,12 +40,10 @@
     <t>Fiber 3 Power (dBm.)</t>
   </si>
   <si>
-    <t>Fiber 4
- Wavelength (nm.)</t>
-  </si>
-  <si>
-    <t>Fiber 4
- Power (dBm.)</t>
+    <t>Fiber 4 Wavelength (nm.)</t>
+  </si>
+  <si>
+    <t>Fiber 4 Power (dBm.)</t>
   </si>
   <si>
     <t>Mean Temp (K)</t>
@@ -60,8 +58,7 @@
     <t>Fiber 3 Δλ, from start (nm.)</t>
   </si>
   <si>
-    <t>Fiber 4
- Δλ, from start (nm.)</t>
+    <t>Fiber 4 Δλ, from start (nm.)</t>
   </si>
   <si>
     <t>ΔT, from start (K)</t>
@@ -8898,7 +8895,7 @@
         <v>0</v>
       </c>
       <c r="D107" s="7">
-        <f>VALUE(-10.45)</f>
+        <f>VALUE(-20.0)</f>
         <v>0</v>
       </c>
       <c r="E107" s="8">

</xml_diff>